<commit_message>
correct 229v1 growth rates
</commit_message>
<xml_diff>
--- a/data/GrowthRates/GrowthRates.xlsx
+++ b/data/GrowthRates/GrowthRates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="#2229v1" sheetId="1" state="visible" r:id="rId2"/>
@@ -256,11 +256,11 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -304,7 +304,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>1</v>
+        <v>15.5</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>8.1</v>
@@ -321,7 +321,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>2</v>
+        <v>17.25</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>16.3333333333333</v>
@@ -335,7 +335,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>3</v>
+        <v>19.25</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>18</v>
@@ -352,7 +352,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>4</v>
+        <v>21.25</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>23.3333333333333</v>
@@ -369,7 +369,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>5</v>
+        <v>23.25</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>23.3333333333333</v>
@@ -386,7 +386,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>6</v>
+        <v>25.25</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>25.3333333333333</v>
@@ -403,7 +403,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>7</v>
+        <v>42.25</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>35.3333333333333</v>
@@ -420,7 +420,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>37.3333333333333</v>
@@ -437,7 +437,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>40.6666666666667</v>
@@ -454,7 +454,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>30.3333333333333</v>
@@ -471,7 +471,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>11</v>
+        <v>66.25</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>22.3333333333333</v>
@@ -505,10 +505,10 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D2:D13 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -823,11 +823,11 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D13 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1143,10 +1143,10 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D2:D13 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1462,10 +1462,10 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D13 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
growth experiment LenaDaniel, Wierckx
</commit_message>
<xml_diff>
--- a/data/GrowthRates/GrowthRates.xlsx
+++ b/data/GrowthRates/GrowthRates.xlsx
@@ -13,6 +13,10 @@
     <sheet name="MasterLV3_130v2" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="MasterLV3_200v1" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="MasterLV3_200v2" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="2112_GP10glc" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="2112_GP20glc" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="2112_GP50glc" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="2112_GP10glc_5ace" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="53">
   <si>
     <t xml:space="preserve">Metadata: Key</t>
   </si>
@@ -132,16 +136,68 @@
   </si>
   <si>
     <t xml:space="preserve">200-[2.6-2.4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM_Rep1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM_Rep2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM_Rep3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub_Rep1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub_Rep2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub_Rep3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12gp10glc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc_Rep1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc_Rep2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc_Rep3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ace_Rep1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ace_Rep2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ace_Rep3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,6 +231,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -220,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,6 +297,18 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -257,10 +331,10 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -505,10 +579,10 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D2:D13 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -824,10 +898,10 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1143,10 +1217,10 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D2:D13 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1462,10 +1536,10 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1758,6 +1832,2536 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="lena.ullmann@rwth-aachen.de"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J91"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>8.8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false" t="array" ref="H5:J7">0</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="lena.ullmann@rwth-aachen.de"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J91"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>88</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>81</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>81</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="lena.ullmann@rwth-aachen.de"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J91"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>48.4</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>114</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>101</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="lena.ullmann@rwth-aachen.de"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M91"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="K2" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="M2" s="6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="K3" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>3.26</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M4" s="6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>2766</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Wierckx growth rate analysis
</commit_message>
<xml_diff>
--- a/data/GrowthRates/GrowthRates.xlsx
+++ b/data/GrowthRates/GrowthRates.xlsx
@@ -5,18 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="#2229v1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="MasterLV3_130v1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="MasterLV3_130v2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="MasterLV3_200v1" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="MasterLV3_200v2" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="LV3_130v1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="LV3_130v2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="LV3_200v1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="LV3_200v2" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="2112_GP10glc" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="2112_GP20glc" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="2112_GP50glc" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="2112_GP10glc_5ace" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Wierckx_50glc" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Wierckx_100glc" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="61">
   <si>
     <t xml:space="preserve">Metadata: Key</t>
   </si>
@@ -187,6 +189,30 @@
   </si>
   <si>
     <t xml:space="preserve">Acetate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wierckx_50glc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philipp Ernst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.ernst@fz-juelich.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U. maydis MB215 K3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 mM MES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.3390/jof7010020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wierckx_100glc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66g/l CaCO3</t>
   </si>
 </sst>
 </file>
@@ -330,11 +356,11 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -564,6 +590,1062 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J91"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>54.86544</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>53.03862</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>54.53082</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1.085</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1.482</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>48.00366</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>48.43548</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>47.48706</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>12.089</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>12.159</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>12.784</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>30.82662</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>31.71222</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>32.97708</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>17.676</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>17.887</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>17.697</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>21.29004</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>21.63006</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>21.99024</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>21.547</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>21.505</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>21.82</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>16.47324</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>16.13718</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>16.371</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>24.119</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>23.146</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>23.161</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>9.89748</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>9.38106</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>9.45954</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="5"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="5"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="5"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="5"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E85" s="5"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="5"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="5"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="5"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" display="https://doi.org/10.3390/jof7010020"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J91"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>110.7499</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>115.7674</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>113.8973</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1.268</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.911</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>104.9792</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>109.3342</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>104.9839</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>10.068</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>9.929</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>9.935</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>93.15</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>93.2409</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>90.81288</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>16.84</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>17.498</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>16.872</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>78.60726</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>78.81696</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>76.04604</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>26.574</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>23.817</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>24.27</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>66.40902</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>63.42102</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>66.17772</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>34.034</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>33.285</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>34.132</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>56.19114</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>55.64286</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>53.99118</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="5"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="5"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="5"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="5"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E85" s="5"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="5"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="5"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="5"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" display="https://doi.org/10.3390/jof7010020"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -582,7 +1664,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -901,7 +1983,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1220,7 +2302,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1535,11 +2617,11 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1858,7 +2940,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1867,25 +2949,25 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1908,13 +2990,13 @@
       <c r="G2" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1937,13 +3019,13 @@
       <c r="G3" s="4" t="n">
         <v>1.4</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>8.7</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>9.1</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>8.8</v>
       </c>
     </row>
@@ -1966,13 +3048,13 @@
       <c r="G4" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="n">
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1980,7 +3062,7 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="4" t="n">
@@ -1995,14 +3077,14 @@
       <c r="G5" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <f aca="false" t="array" ref="H5:J7">0</f>
         <v>0</v>
       </c>
-      <c r="I5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="0" t="n">
+      <c r="I5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2025,13 +3107,13 @@
       <c r="G6" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2054,13 +3136,13 @@
       <c r="G7" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0" t="n">
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2085,10 +3167,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E10" s="5"/>
@@ -2468,10 +3550,10 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2480,25 +3562,25 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2521,13 +3603,13 @@
       <c r="G2" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -2550,13 +3632,13 @@
       <c r="G3" s="4" t="n">
         <v>1.24</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>17.3</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>17.5</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>18.2</v>
       </c>
     </row>
@@ -2579,13 +3661,13 @@
       <c r="G4" s="4" t="n">
         <v>29.5</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>3.4</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>3.5</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>3.6</v>
       </c>
     </row>
@@ -2593,7 +3675,7 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="4" t="n">
@@ -2608,13 +3690,13 @@
       <c r="G5" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>2.9</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>3.1</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="1" t="n">
         <v>2.9</v>
       </c>
     </row>
@@ -2637,13 +3719,13 @@
       <c r="G6" s="4" t="n">
         <v>81</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2666,13 +3748,13 @@
       <c r="G7" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0" t="n">
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2697,10 +3779,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E10" s="5"/>
@@ -3083,7 +4165,7 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3092,25 +4174,25 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3205,7 +4287,7 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="4" t="n">
@@ -3309,10 +4391,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E10" s="5"/>
@@ -3695,7 +4777,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3704,34 +4786,34 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3853,7 +4935,7 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="4" t="n">
@@ -3984,10 +5066,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E10" s="5"/>
@@ -3997,7 +5079,7 @@
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E11" s="5"/>
@@ -4007,17 +5089,17 @@
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E13" s="5"/>

</xml_diff>

<commit_message>
add new analysis 220204
</commit_message>
<xml_diff>
--- a/data/GrowthRates/GrowthRates.xlsx
+++ b/data/GrowthRates/GrowthRates.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="#2229v1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="2229v1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="LV3_130v1" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="LV3_130v2" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="LV3_200v1" sheetId="4" state="visible" r:id="rId5"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="64">
   <si>
     <t xml:space="preserve">Metadata: Key</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#2229</t>
   </si>
   <si>
     <t xml:space="preserve">Contact</t>
@@ -370,10 +367,10 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -396,8 +393,8 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+      <c r="B2" s="1" t="n">
+        <v>2229</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -411,10 +408,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>15.5</v>
@@ -428,10 +425,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>17.25</v>
@@ -445,7 +442,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>19.25</v>
@@ -459,10 +456,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>21.25</v>
@@ -476,10 +473,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>23.25</v>
@@ -496,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>25.25</v>
@@ -510,10 +507,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>42.25</v>
@@ -527,10 +524,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>45</v>
@@ -544,10 +541,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>48</v>
@@ -561,10 +558,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>51</v>
@@ -578,10 +575,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>66.25</v>
@@ -621,7 +618,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -634,31 +631,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -666,7 +663,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
@@ -701,10 +698,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>5.25</v>
@@ -739,10 +736,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>23.5</v>
@@ -777,10 +774,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>27</v>
@@ -815,10 +812,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>47</v>
@@ -853,10 +850,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>63</v>
@@ -894,24 +891,24 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>10</v>
@@ -924,24 +921,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>5</v>
@@ -951,47 +948,47 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1"/>
       <c r="E18" s="4"/>
@@ -1314,7 +1311,7 @@
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1327,22 +1324,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,7 +1347,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
@@ -1376,10 +1373,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>24</v>
@@ -1405,10 +1402,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>48</v>
@@ -1434,7 +1431,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1"/>
       <c r="D5" s="0" t="n">
@@ -1461,10 +1458,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>96</v>
@@ -1490,10 +1487,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>120</v>
@@ -1522,22 +1519,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>50</v>
@@ -1546,46 +1543,46 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="4"/>
     </row>
@@ -1842,7 +1839,7 @@
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1855,22 +1852,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1875,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
@@ -1904,10 +1901,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>24</v>
@@ -1933,10 +1930,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>48</v>
@@ -1962,7 +1959,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1"/>
       <c r="D5" s="0" t="n">
@@ -1989,10 +1986,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>96</v>
@@ -2018,10 +2015,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>117</v>
@@ -2050,22 +2047,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>100</v>
@@ -2074,46 +2071,46 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="4"/>
     </row>
@@ -2370,7 +2367,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2386,13 +2383,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +2397,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -2420,10 +2417,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>22</v>
@@ -2443,10 +2440,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>48</v>
@@ -2466,7 +2463,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>68</v>
@@ -2486,10 +2483,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>95</v>
@@ -2509,10 +2506,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>120</v>
@@ -2535,7 +2532,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>168</v>
@@ -2555,10 +2552,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>192</v>
@@ -2578,10 +2575,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>214</v>
@@ -2601,10 +2598,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>237</v>
@@ -2624,10 +2621,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>264</v>
@@ -2647,18 +2644,18 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2689,7 +2686,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2705,13 +2702,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,7 +2716,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -2739,10 +2736,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>22</v>
@@ -2762,10 +2759,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>48</v>
@@ -2785,7 +2782,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>68</v>
@@ -2805,10 +2802,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>95</v>
@@ -2828,10 +2825,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>120</v>
@@ -2854,7 +2851,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>168</v>
@@ -2874,10 +2871,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>192</v>
@@ -2897,10 +2894,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>214</v>
@@ -2920,10 +2917,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>237</v>
@@ -2943,10 +2940,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>264</v>
@@ -2966,18 +2963,18 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,7 +3005,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3024,13 +3021,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3038,7 +3035,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -3058,10 +3055,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>22</v>
@@ -3081,10 +3078,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>48</v>
@@ -3104,7 +3101,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>68</v>
@@ -3124,10 +3121,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>95</v>
@@ -3147,10 +3144,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>120</v>
@@ -3173,7 +3170,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>168</v>
@@ -3193,10 +3190,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>192</v>
@@ -3216,10 +3213,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>214</v>
@@ -3239,10 +3236,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>237</v>
@@ -3262,10 +3259,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>264</v>
@@ -3285,18 +3282,18 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3327,7 +3324,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3343,13 +3340,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3357,7 +3354,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -3377,10 +3374,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>22</v>
@@ -3400,10 +3397,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>48</v>
@@ -3423,7 +3420,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>68</v>
@@ -3443,10 +3440,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>95</v>
@@ -3466,10 +3463,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>120</v>
@@ -3492,7 +3489,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>168</v>
@@ -3512,10 +3509,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>192</v>
@@ -3535,10 +3532,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>214</v>
@@ -3558,10 +3555,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>237</v>
@@ -3581,10 +3578,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>264</v>
@@ -3604,18 +3601,18 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3640,13 +3637,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3662,13 +3659,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -3677,7 +3674,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
@@ -3697,13 +3694,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="0" t="n">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.846666666666667</v>
@@ -3720,13 +3717,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" s="0" t="n">
-        <v>4</v>
+        <v>4.01</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0.873333333333333</v>
@@ -3743,11 +3740,11 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1"/>
       <c r="D5" s="0" t="n">
-        <v>6</v>
+        <v>6.01</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0.946666666666667</v>
@@ -3764,13 +3761,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>8</v>
+        <v>8.01</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1.08</v>
@@ -3787,13 +3784,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D7" s="0" t="n">
-        <v>10</v>
+        <v>10.01</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1.42</v>
@@ -3813,7 +3810,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>12</v>
@@ -3833,13 +3830,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="0" t="n">
-        <v>24</v>
+        <v>24.01</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>35</v>
@@ -3856,13 +3853,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>20</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>28</v>
+        <v>28.01</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>49</v>
@@ -3879,13 +3876,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D11" s="0" t="n">
-        <v>32</v>
+        <v>32.01</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>44</v>
@@ -3902,13 +3899,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>49</v>
+        <v>49.01</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>39.6666666666667</v>
@@ -3925,25 +3922,25 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2"/>
       <c r="E15" s="4"/>
@@ -4172,9 +4169,6 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="4"/>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E91" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4201,7 +4195,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4214,22 +4208,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4237,7 +4231,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
@@ -4263,10 +4257,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>5.25</v>
@@ -4292,10 +4286,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>23.5</v>
@@ -4321,10 +4315,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>27</v>
@@ -4351,10 +4345,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>47</v>
@@ -4380,10 +4374,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>63</v>
@@ -4412,24 +4406,24 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>10</v>
@@ -4439,47 +4433,47 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="4"/>
@@ -4814,7 +4808,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4827,22 +4821,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4850,7 +4844,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
@@ -4876,10 +4870,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>5.25</v>
@@ -4905,10 +4899,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>23.5</v>
@@ -4934,10 +4928,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>27</v>
@@ -4963,10 +4957,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>47</v>
@@ -4992,10 +4986,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>63</v>
@@ -5024,24 +5018,24 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>20</v>
@@ -5051,47 +5045,47 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="4"/>
@@ -5426,7 +5420,7 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5439,22 +5433,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5462,7 +5456,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
@@ -5488,10 +5482,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>5.25</v>
@@ -5517,10 +5511,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>23.5</v>
@@ -5546,10 +5540,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>27</v>
@@ -5575,10 +5569,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>47</v>
@@ -5604,10 +5598,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>63</v>
@@ -5636,24 +5630,24 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>20</v>
@@ -5663,47 +5657,47 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="4"/>

</xml_diff>

<commit_message>
add medium, strain growth experiments
</commit_message>
<xml_diff>
--- a/data/GrowthRates/GrowthRates.xlsx
+++ b/data/GrowthRates/GrowthRates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2229v1" sheetId="1" state="visible" r:id="rId2"/>
@@ -71,13 +71,13 @@
     <t xml:space="preserve">Strain</t>
   </si>
   <si>
-    <t xml:space="preserve">U. maydis …</t>
+    <t xml:space="preserve">U. maydis MB215</t>
   </si>
   <si>
     <t xml:space="preserve">Media</t>
   </si>
   <si>
-    <t xml:space="preserve">Minimal</t>
+    <t xml:space="preserve">Minimal Modified Tabuchi</t>
   </si>
   <si>
     <t xml:space="preserve">Glucose</t>
@@ -119,9 +119,6 @@
     <t xml:space="preserve">130-[0-1]</t>
   </si>
   <si>
-    <t xml:space="preserve">Minimal?</t>
-  </si>
-  <si>
     <t xml:space="preserve">OD600</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t xml:space="preserve">LV11_glc20</t>
   </si>
   <si>
-    <t xml:space="preserve">U. maydis</t>
-  </si>
-  <si>
     <t xml:space="preserve">Concentration</t>
   </si>
   <si>
@@ -162,6 +156,9 @@
   </si>
   <si>
     <t xml:space="preserve">2196_glyc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U. maydis FB21</t>
   </si>
   <si>
     <t xml:space="preserve">Glycerol</t>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t xml:space="preserve">ace_Rep3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U. maydis …</t>
   </si>
   <si>
     <t xml:space="preserve">Acetate</t>
@@ -380,11 +380,11 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -629,10 +629,10 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -645,22 +645,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
@@ -755,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>27</v>
@@ -784,7 +784,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>47</v>
@@ -813,7 +813,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>63</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>20</v>
@@ -882,7 +882,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -892,7 +892,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -909,7 +909,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="4"/>
@@ -1241,10 +1241,10 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1257,22 +1257,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,7 +1280,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>27</v>
@@ -1396,7 +1396,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>47</v>
@@ -1425,7 +1425,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>63</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>20</v>
@@ -1494,7 +1494,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1504,7 +1504,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="4"/>
@@ -1853,10 +1853,10 @@
   <dimension ref="A1:M91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1869,31 +1869,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,7 +1901,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
@@ -2015,7 +2015,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>27</v>
@@ -2053,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>47</v>
@@ -2091,7 +2091,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>63</v>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>10</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>5</v>
@@ -2199,7 +2199,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -2209,7 +2209,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1"/>
       <c r="E18" s="4"/>
@@ -2546,10 +2546,10 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2562,22 +2562,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,7 +2772,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>50</v>
@@ -2811,13 +2811,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>65</v>
@@ -3074,10 +3074,10 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3090,22 +3090,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3300,7 +3300,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>100</v>
@@ -3339,13 +3339,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>65</v>
@@ -3602,10 +3602,10 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3747,7 +3747,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>120</v>
@@ -3839,7 +3839,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>237</v>
@@ -3890,10 +3890,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,7 +3924,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3954,7 +3954,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -4066,7 +4066,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>120</v>
@@ -4158,7 +4158,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>237</v>
@@ -4209,10 +4209,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4240,10 +4240,10 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4273,7 +4273,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -4385,7 +4385,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>120</v>
@@ -4477,7 +4477,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>237</v>
@@ -4528,10 +4528,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4559,10 +4559,10 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4592,7 +4592,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -4704,7 +4704,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>120</v>
@@ -4796,7 +4796,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>237</v>
@@ -4847,10 +4847,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4878,10 +4878,10 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4897,13 +4897,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -4912,7 +4912,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
@@ -5002,7 +5002,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>8.01</v>
@@ -5091,7 +5091,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>20</v>
@@ -5172,13 +5172,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2"/>
       <c r="E15" s="4"/>
@@ -5429,11 +5429,11 @@
   </sheetPr>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5449,16 +5449,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1"/>
     </row>
@@ -5467,7 +5467,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
@@ -5569,7 +5569,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>24</v>
@@ -5670,7 +5670,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>20</v>
@@ -5706,13 +5706,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2"/>
       <c r="E15" s="4"/>
@@ -5964,10 +5964,10 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5983,16 +5983,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1"/>
     </row>
@@ -6001,7 +6001,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
@@ -6103,7 +6103,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>24</v>
@@ -6155,7 +6155,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>43</v>
@@ -6204,7 +6204,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>2</v>
@@ -6294,13 +6294,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2"/>
       <c r="E15" s="4"/>
@@ -6555,7 +6555,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6568,22 +6568,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6591,7 +6591,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0</v>
@@ -6678,7 +6678,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>27</v>
@@ -6708,7 +6708,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>47</v>
@@ -6737,7 +6737,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>63</v>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>10</v>
@@ -6806,7 +6806,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -6816,7 +6816,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -6833,7 +6833,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="4"/>

</xml_diff>